<commit_message>
improve UI/UX for pages
</commit_message>
<xml_diff>
--- a/public/templates/mau-nhap-mon-hoc.xlsx
+++ b/public/templates/mau-nhap-mon-hoc.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DU AN QUAN LY SINH VIEN VA KET QUA HOC TAP\Frontend\free-nextjs-admin-dashboard-main\public\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{222F9384-CFEE-4C22-8BDB-D971EDA2416C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B55D0A2D-AA42-4C6C-A926-D7D1738C0F4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="38">
   <si>
     <t>STT</t>
   </si>
@@ -34,9 +34,6 @@
     <t>CHUYEN_NGANH</t>
   </si>
   <si>
-    <t>GV101</t>
-  </si>
-  <si>
     <t>MH02</t>
   </si>
   <si>
@@ -46,36 +43,24 @@
     <t>TU_CHON</t>
   </si>
   <si>
-    <t>GV102</t>
-  </si>
-  <si>
     <t>MH03</t>
   </si>
   <si>
     <t>Lập trình hướng đối tượng</t>
   </si>
   <si>
-    <t>GV103</t>
-  </si>
-  <si>
     <t>MH04</t>
   </si>
   <si>
     <t>Mạng máy tính</t>
   </si>
   <si>
-    <t>GV104</t>
-  </si>
-  <si>
     <t>MH05</t>
   </si>
   <si>
     <t>Cơ sở dữ liệu</t>
   </si>
   <si>
-    <t>GV105</t>
-  </si>
-  <si>
     <t>MH06</t>
   </si>
   <si>
@@ -85,90 +70,60 @@
     <t>DAI_CUONG</t>
   </si>
   <si>
-    <t>GV106</t>
-  </si>
-  <si>
     <t>MH07</t>
   </si>
   <si>
     <t>Trí tuệ nhân tạo</t>
   </si>
   <si>
-    <t>GV107</t>
-  </si>
-  <si>
     <t>MH08</t>
   </si>
   <si>
     <t>Hệ điều hành</t>
   </si>
   <si>
-    <t>GV108</t>
-  </si>
-  <si>
     <t>MH09</t>
   </si>
   <si>
     <t>Học máy</t>
   </si>
   <si>
-    <t>GV109</t>
-  </si>
-  <si>
     <t>MH10</t>
   </si>
   <si>
     <t>An toàn thông tin</t>
   </si>
   <si>
-    <t>GV110</t>
-  </si>
-  <si>
     <t>MH11</t>
   </si>
   <si>
     <t>Kỹ năng mềm</t>
   </si>
   <si>
-    <t>GV111</t>
-  </si>
-  <si>
     <t>MH12</t>
   </si>
   <si>
     <t>Phương pháp nghiên cứu khoa học</t>
   </si>
   <si>
-    <t>GV112</t>
-  </si>
-  <si>
     <t>MH13</t>
   </si>
   <si>
     <t>Điện toán đám mây</t>
   </si>
   <si>
-    <t>GV113</t>
-  </si>
-  <si>
     <t>MH14</t>
   </si>
   <si>
     <t>Phát triển ứng dụng Web</t>
   </si>
   <si>
-    <t>GV114</t>
-  </si>
-  <si>
     <t>MH15</t>
   </si>
   <si>
     <t>Phát triển ứng dụng di động</t>
   </si>
   <si>
-    <t>GV115</t>
-  </si>
-  <si>
     <t>Số tín chỉ (Required)</t>
   </si>
   <si>
@@ -179,9 +134,6 @@
   </si>
   <si>
     <t>Mã Môn học (Required)</t>
-  </si>
-  <si>
-    <t>Mã Giảng viên phụ trách  (Optional)</t>
   </si>
 </sst>
 </file>
@@ -244,7 +196,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -254,9 +206,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -560,10 +509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -573,30 +522,26 @@
     <col min="3" max="3" width="49.5703125" customWidth="1"/>
     <col min="4" max="4" width="42.140625" customWidth="1"/>
     <col min="5" max="5" width="27.7109375" customWidth="1"/>
-    <col min="6" max="6" width="38.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -612,59 +557,50 @@
       <c r="E2" s="2">
         <v>2</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>7</v>
       </c>
       <c r="E3" s="2">
         <v>4</v>
       </c>
-      <c r="F3" s="4" t="s">
+    </row>
+    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>3</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>10</v>
-      </c>
       <c r="D4" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E4" s="2">
         <v>3</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>3</v>
@@ -672,19 +608,16 @@
       <c r="E5" s="2">
         <v>3</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>3</v>
@@ -692,139 +625,118 @@
       <c r="E6" s="2">
         <v>4</v>
       </c>
-      <c r="F6" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E7" s="2">
         <v>3</v>
       </c>
-      <c r="F7" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E8" s="2">
         <v>2</v>
       </c>
-      <c r="F8" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E9" s="2">
         <v>2</v>
       </c>
-      <c r="F9" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E10" s="2">
         <v>2</v>
       </c>
-      <c r="F10" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E11" s="2">
         <v>3</v>
       </c>
-      <c r="F11" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E12" s="2">
         <v>4</v>
       </c>
-      <c r="F12" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>3</v>
@@ -832,68 +744,56 @@
       <c r="E13" s="2">
         <v>4</v>
       </c>
-      <c r="F13" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E14" s="2">
         <v>2</v>
       </c>
-      <c r="F14" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E15" s="2">
         <v>4</v>
       </c>
-      <c r="F15" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E16" s="2">
         <v>3</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>